<commit_message>
update FPList first level
</commit_message>
<xml_diff>
--- a/FPListFirstLevelT_0001.xlsx
+++ b/FPListFirstLevelT_0001.xlsx
@@ -5,24 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuchaow/Documents/GitHub/RStudio/thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuchaow/Documents/GitHub/RStudio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1814F2F-0C62-6547-8140-DB4C2168CE5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36567F2E-B020-C847-949D-0067523621C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="460" windowWidth="39880" windowHeight="21380" activeTab="2" xr2:uid="{9A1069F4-AA40-B645-B99F-CD91542F68D9}"/>
+    <workbookView xWindow="3760" yWindow="460" windowWidth="39880" windowHeight="21380" xr2:uid="{9A1069F4-AA40-B645-B99F-CD91542F68D9}"/>
   </bookViews>
   <sheets>
     <sheet name="NiftiList" sheetId="1" r:id="rId1"/>
     <sheet name="DHOG_Reg" sheetId="2" r:id="rId2"/>
     <sheet name="DMOG_Reg" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">DMOG_Reg!$E$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">DMOG_Reg!$E$2:$E$510</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">DMOG_Reg!$F$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">DMOG_Reg!$F$2:$F$510</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="421">
   <si>
     <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S01/SPMemoOutputs/spmT_0001.nii   '</t>
   </si>
@@ -672,6 +666,630 @@
   </si>
   <si>
     <t>DMOG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S01/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S01/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S01/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S01/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S02/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S02/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S02/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S02/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S03/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S03/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S03/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S03/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S04/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S04/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S04/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S04/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S05/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S05/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S05/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S05/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S06/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S06/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S06/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S06/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S08/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S08/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S08/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S08/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S09/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S09/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S09/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S09/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S10/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S10/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S10/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S10/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S12/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S12/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S12/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S12/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S14/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S14/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S14/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S14/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S15/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S15/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S15/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S15/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S16/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S16/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S16/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S16/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S17/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S17/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S17/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S17/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S19/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S19/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S19/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S19/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S20/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S20/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S20/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S20/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S21/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S21/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S21/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S21/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S22/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S22/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S22/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S22/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S23/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S23/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S23/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S23/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S24/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S24/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S24/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S24/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S25/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S25/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S25/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S25/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S26/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S26/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S26/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S26/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S27/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S27/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S27/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S27/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S28/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S28/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S28/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S28/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S29/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S29/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S29/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S29/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S30/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S30/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S30/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S30/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S31/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S31/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S31/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S31/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S32/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S32/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S32/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S32/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S33/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S33/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S33/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S33/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S34/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S34/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S34/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S34/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S35/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S35/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S35/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S35/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S37/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S37/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S37/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S37/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S38/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S38/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S38/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S38/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S39/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S39/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S39/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S39/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S40/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S40/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S40/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S40/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S41/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S41/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S41/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S41/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S42/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S42/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S42/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S42/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S43/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S43/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S43/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S43/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S44/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S44/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S44/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S44/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S46/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S46/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S46/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S46/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S47/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S47/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S47/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S47/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S48/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S48/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S48/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S48/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S49/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S49/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S49/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S49/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S50/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S50/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S50/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S50/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S51/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S51/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S51/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S51/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S53/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S53/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S53/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S53/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S55/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S55/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S55/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S55/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S56/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S56/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S56/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S56/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S57/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S57/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S57/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S57/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S58/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S58/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S58/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S58/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S59/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S59/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S59/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S59/SPMlitOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S60/SPMemoOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S60/SPMemoOutputs128/con_0001.nii'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S60/SPMlitOutputs/con_0001.nii   '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '/Users/yuchaow/Documents/narrativefMRIdata/S60/SPMlitOutputs128/con_0001.nii'</t>
   </si>
 </sst>
 </file>
@@ -714,7 +1332,217 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="31">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB4C6E7"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6E0B4"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB4C6E7"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6E0B4"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB4C6E7"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6E0B4"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="0"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="0"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="0"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="0"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -746,38 +1574,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9E1F2"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -17586,1076 +18382,1720 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35DF6DA-8736-A044-B977-398B6DFD04AB}">
-  <dimension ref="A1:A208"/>
+  <dimension ref="A1:D208"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="80" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D75" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D77" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D78" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D79" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D80" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D81" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D83" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D84" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D87" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D92" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D101" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D102" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D103" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D104" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D105" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D106" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D107" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D108" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D109" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D110" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D111" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D112" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D113" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D114" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D115" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D116" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D117" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D118" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D119" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D120" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D121" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D122" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D123" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D124" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D125" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D126" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D127" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D128" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D129" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D130" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D131" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D132" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D133" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D134" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D135" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D136" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D137" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D138" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D139" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D140" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D141" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D142" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D143" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D144" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D145" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D146" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D147" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D148" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D149" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D150" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D151" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D152" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D153" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D154" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D155" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D156" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D157" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D158" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D159" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D160" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D161" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D162" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D163" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D164" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D165" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D166" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D167" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D168" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D169" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D170" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D171" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D172" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D173" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D174" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D175" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D176" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D177" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D178" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D179" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D180" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D181" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D182" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D183" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D184" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D185" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D186" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D187" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D188" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D189" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D190" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D191" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D192" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D193" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D194" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D195" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D196" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D197" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D198" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D199" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D200" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D201" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D202" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D203" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D204" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D205" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D206" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D207" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>206</v>
       </c>
+      <c r="D208" t="s">
+        <v>419</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A212">
-    <sortCondition sortBy="cellColor" ref="A1:A212" dxfId="7"/>
-    <sortCondition sortBy="cellColor" ref="A1:A212" dxfId="6"/>
-    <sortCondition sortBy="cellColor" ref="A1:A212" dxfId="5"/>
-    <sortCondition sortBy="cellColor" ref="A1:A212" dxfId="4"/>
+  <sortState ref="D1:D208">
+    <sortCondition sortBy="cellColor" ref="D1:D208" dxfId="7"/>
+    <sortCondition sortBy="cellColor" ref="D1:D208" dxfId="6"/>
+    <sortCondition sortBy="cellColor" ref="D1:D208" dxfId="5"/>
+    <sortCondition sortBy="cellColor" ref="D1:D208" dxfId="4"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="litOutputs/spm">
+    <cfRule type="containsText" dxfId="26" priority="6" operator="containsText" text="litOutputs/spm">
       <formula>NOT(ISERROR(SEARCH("litOutputs/spm",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="emoOutputs/spm">
+    <cfRule type="containsText" dxfId="25" priority="7" operator="containsText" text="emoOutputs/spm">
       <formula>NOT(ISERROR(SEARCH("emoOutputs/spm",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="litOutputs128">
+    <cfRule type="containsText" dxfId="24" priority="8" operator="containsText" text="litOutputs128">
       <formula>NOT(ISERROR(SEARCH("litOutputs128",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="emoOutputs128">
+    <cfRule type="containsText" dxfId="23" priority="9" operator="containsText" text="emoOutputs128">
       <formula>NOT(ISERROR(SEARCH("emoOutputs128",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1">
+    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="emoOutputs128/con">
+      <formula>NOT(ISERROR(SEARCH("emoOutputs128/con",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="emoOutputs128/con">
+      <formula>NOT(ISERROR(SEARCH("emoOutputs128/con",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="litOutputs128/con">
+      <formula>NOT(ISERROR(SEARCH("litOutputs128/con",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="emoOutputs/con">
+      <formula>NOT(ISERROR(SEARCH("emoOutputs/con",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="litOutputs/con">
+      <formula>NOT(ISERROR(SEARCH("litOutputs/con",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26292,7 +27732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11C3CA7-AC98-E04D-AE4D-E674EBFDE6CD}">
   <dimension ref="A1:F510"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>

</xml_diff>